<commit_message>
figures of basic relationships between targets and between surrogates; coral cover and coral richness over time
</commit_message>
<xml_diff>
--- a/taxa_checked.xlsx
+++ b/taxa_checked.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="576" windowWidth="8004" windowHeight="8736" activeTab="4"/>
+    <workbookView xWindow="960" yWindow="576" windowWidth="8004" windowHeight="8736" firstSheet="4" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="fish_taxa" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="coral_taxa" sheetId="3" r:id="rId3"/>
     <sheet name="fish_taxa_rearranged" sheetId="4" r:id="rId4"/>
     <sheet name="all_taxa" sheetId="5" r:id="rId5"/>
+    <sheet name="Corals and Sponges re-arranged" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1085" uniqueCount="359">
   <si>
     <t>doctorfish</t>
   </si>
@@ -1026,6 +1027,75 @@
   </si>
   <si>
     <t>Maybe "Ircinia smooth" or Spongia</t>
+  </si>
+  <si>
+    <t>Higginsia coralloides (may include Ptilocaulis walpersii)</t>
+  </si>
+  <si>
+    <t>Agaricia spp. (mostly Agaricia humilis</t>
+  </si>
+  <si>
+    <t>Niphates erecta (may include</t>
+  </si>
+  <si>
+    <t>Neopetrosia proxima (may include</t>
+  </si>
+  <si>
+    <t>Higginsia coralloides (may include</t>
+  </si>
+  <si>
+    <t>Like Callyspongia fallax but soft with</t>
+  </si>
+  <si>
+    <t>Breadcrumb (Calyx podatypa, Svenzea</t>
+  </si>
+  <si>
+    <t>Aplysina lacunosa, Suberea sp., and</t>
+  </si>
+  <si>
+    <t>Aplysina fistularis, Aplysina fulva, and</t>
+  </si>
+  <si>
+    <t>Amphimedon sp. (maybe Amphimedon</t>
+  </si>
+  <si>
+    <t>Agelas citrina, Agelas clathrodes, or</t>
+  </si>
+  <si>
+    <t>Montastraea annularis, M. franksi, M. faveolata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Xestospongia subtriangularis)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Niphates amorpha)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Ptilocaulis walpersii)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   pinched tube ends</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   cristinae, or Svenzea zeai)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Verongula reiswigi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Aplysina insularis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   (genus name now Orbicella)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   and Agaricia lamarcki)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   complanata)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Clathria faviformis</t>
   </si>
 </sst>
 </file>
@@ -1251,7 +1321,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1437,6 +1507,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -1618,7 +1694,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1723,6 +1799,11 @@
     <xf numFmtId="0" fontId="18" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="26" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3042,8 +3123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B59"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A40" sqref="A1:A1048576"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3258,7 +3339,7 @@
     </row>
     <row r="35" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="44" t="s">
-        <v>267</v>
+        <v>336</v>
       </c>
       <c r="B35" s="23"/>
     </row>
@@ -5230,7 +5311,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B33" workbookViewId="0">
+    <sheetView topLeftCell="B33" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:F60"/>
     </sheetView>
   </sheetViews>
@@ -6389,4 +6470,498 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B68"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A3" sqref="A1:B68"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="42.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="39.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="40" t="s">
+        <v>298</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="41" t="s">
+        <v>300</v>
+      </c>
+      <c r="B2" s="51" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="41" t="s">
+        <v>299</v>
+      </c>
+      <c r="B3" s="51" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="42" t="s">
+        <v>301</v>
+      </c>
+      <c r="B4" s="44" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="50" t="s">
+        <v>337</v>
+      </c>
+      <c r="B5" s="44" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="50" t="s">
+        <v>356</v>
+      </c>
+      <c r="B6" s="44" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="42" t="s">
+        <v>315</v>
+      </c>
+      <c r="B7" s="44" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="42" t="s">
+        <v>306</v>
+      </c>
+      <c r="B8" s="51" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="42" t="s">
+        <v>302</v>
+      </c>
+      <c r="B9" s="51" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="42" t="s">
+        <v>304</v>
+      </c>
+      <c r="B10" s="44" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="24" t="s">
+        <v>327</v>
+      </c>
+      <c r="B11" s="51" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="42" t="s">
+        <v>311</v>
+      </c>
+      <c r="B12" s="51" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="25" t="s">
+        <v>308</v>
+      </c>
+      <c r="B13" s="44" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="42" t="s">
+        <v>303</v>
+      </c>
+      <c r="B14" s="51" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="39" t="s">
+        <v>330</v>
+      </c>
+      <c r="B15" s="51" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="42" t="s">
+        <v>307</v>
+      </c>
+      <c r="B16" s="44" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="42" t="s">
+        <v>312</v>
+      </c>
+      <c r="B17" s="44" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="42" t="s">
+        <v>320</v>
+      </c>
+      <c r="B18" s="51" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="25" t="s">
+        <v>322</v>
+      </c>
+      <c r="B19" s="51" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="42" t="s">
+        <v>305</v>
+      </c>
+      <c r="B20" s="44" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="50" t="s">
+        <v>347</v>
+      </c>
+      <c r="B21" s="51" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="50" t="s">
+        <v>355</v>
+      </c>
+      <c r="B22" s="51" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="42" t="s">
+        <v>310</v>
+      </c>
+      <c r="B23" s="44" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="43" t="s">
+        <v>309</v>
+      </c>
+      <c r="B24" s="44" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="42" t="s">
+        <v>314</v>
+      </c>
+      <c r="B25" s="44" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="44" t="s">
+        <v>323</v>
+      </c>
+      <c r="B26" s="44" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="44" t="s">
+        <v>318</v>
+      </c>
+      <c r="B27" s="44" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="44" t="s">
+        <v>317</v>
+      </c>
+      <c r="B28" s="44" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="44" t="s">
+        <v>324</v>
+      </c>
+      <c r="B29" s="44" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="42" t="s">
+        <v>313</v>
+      </c>
+      <c r="B30" s="44" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="42" t="s">
+        <v>325</v>
+      </c>
+      <c r="B31" s="44" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="24" t="s">
+        <v>316</v>
+      </c>
+      <c r="B32" s="44" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="42" t="s">
+        <v>326</v>
+      </c>
+      <c r="B33" s="44" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="44"/>
+      <c r="B34" s="44" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="44"/>
+      <c r="B35" s="44" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A36" s="44"/>
+      <c r="B36" s="44" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="44"/>
+      <c r="B37" s="44" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="44"/>
+      <c r="B38" s="44" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="44"/>
+      <c r="B39" s="44" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A40" s="44"/>
+      <c r="B40" s="44" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A41" s="44"/>
+      <c r="B41" s="51" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A42" s="44"/>
+      <c r="B42" s="51" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A43" s="44"/>
+      <c r="B43" s="44" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A44" s="44"/>
+      <c r="B44" s="44" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A45" s="44"/>
+      <c r="B45" s="44" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A46" s="44"/>
+      <c r="B46" s="44" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A47" s="44"/>
+      <c r="B47" s="44" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A48" s="44"/>
+      <c r="B48" s="44" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A49" s="44"/>
+      <c r="B49" s="44" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A50" s="44"/>
+      <c r="B50" s="44" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A51" s="44"/>
+      <c r="B51" s="44" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A52" s="44"/>
+      <c r="B52" s="44" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A53" s="44"/>
+      <c r="B53" s="44" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A54" s="44"/>
+      <c r="B54" s="51" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A55" s="44"/>
+      <c r="B55" s="51" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A56" s="44"/>
+      <c r="B56" s="51" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A57" s="44"/>
+      <c r="B57" s="52" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A58" s="44"/>
+      <c r="B58" s="44" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A59" s="44"/>
+      <c r="B59" s="44" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A60" s="44"/>
+      <c r="B60" s="44" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A61" s="44"/>
+      <c r="B61" s="44" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A62" s="44"/>
+      <c r="B62" s="44" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A63" s="44"/>
+      <c r="B63" s="44" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A64" s="44"/>
+      <c r="B64" s="44" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A65" s="44"/>
+      <c r="B65" s="44" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A66" s="44"/>
+      <c r="B66" s="44" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A67" s="44"/>
+      <c r="B67" s="44" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A68" s="44"/>
+      <c r="B68" s="44" t="s">
+        <v>291</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
figures of variables over time and by site for thesis; many file naming, format, and location changes
</commit_message>
<xml_diff>
--- a/taxa_checked.xlsx
+++ b/taxa_checked.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="576" windowWidth="8004" windowHeight="8736" firstSheet="4" activeTab="5"/>
+    <workbookView xWindow="960" yWindow="576" windowWidth="8004" windowHeight="8736" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="fish_taxa" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,15 @@
     <sheet name="fish_taxa_rearranged" sheetId="4" r:id="rId4"/>
     <sheet name="all_taxa" sheetId="5" r:id="rId5"/>
     <sheet name="Corals and Sponges re-arranged" sheetId="6" r:id="rId6"/>
+    <sheet name="Fish italics" sheetId="7" r:id="rId7"/>
+    <sheet name="Corals and Sponges italics" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1085" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1516" uniqueCount="392">
   <si>
     <t>doctorfish</t>
   </si>
@@ -1096,6 +1098,883 @@
   </si>
   <si>
     <t xml:space="preserve">   Clathria faviformis</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Spirastrella coccinea</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Spirastrella hartmani</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Plakortis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> sp.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Niphates</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> sp. or </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Lissodendoryx </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>sp.?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Niphates amorpha</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Niphates erecta</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (may include</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Xestospongia subtriangularis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Neopetrosia proxima</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (may include</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Iotrochota</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> sp.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Hyrtios</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> sp. or </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Spheciospongia vesparium</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Ptilocaulis walpersii</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Higginsia coralloides</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (may include</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Dysidea</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> sp. (maybe etheria)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Cribochalina vasculum</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Petrosia pellasarca</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Like </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Callyspongia fallax</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> but soft with</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>cristinae</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, or </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Svenzea zeai</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Breadcrumb (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Calyx podatypa</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Svenzea</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Artemisina melana</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> or </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Iotrochota arenosa</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Verongula reiswigi</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Aplysina lacunosa</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Suberea</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> sp., and</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Aplysina insularis</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Aplysina fistularis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Aplysina fulva</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, and</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>complanata</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Amphimedon</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> sp. (maybe </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Amphimedon</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Aiolochroia crassa</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Verongula rigida</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Clathria faviformis</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Agelas citrina</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Agelas clathrodes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, or</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Agaricia spp. (mostly </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Agaricia humilis</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">   and </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Agaricia lamarcki</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Diploria strigosa</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Diploria clivosa</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Madracis mirabilis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Madracis decactis</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Montastraea annularis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>M</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>franksi</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>M</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>faveolata</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Mycetophyllia ferox</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Mycetophyllia lamarckiana</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Siderastrea siderea</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Siderastrea radians</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1105,7 +1984,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General_)"/>
   </numFmts>
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="33" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1317,6 +2196,19 @@
       <b/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -1694,7 +2586,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1804,6 +2696,14 @@
     </xf>
     <xf numFmtId="0" fontId="28" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="26" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="31" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="33" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3910,7 +4810,7 @@
   </sheetPr>
   <dimension ref="A1:F118"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C28" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:F1048576"/>
     </sheetView>
   </sheetViews>
@@ -5311,7 +6211,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView topLeftCell="B33" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:F60"/>
     </sheetView>
   </sheetViews>
@@ -6476,8 +7376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A3" sqref="A1:B68"/>
+    <sheetView topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6964,4 +7864,1900 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:F118"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="69.6640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.21875" style="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.44140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" style="26" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5546875" style="26" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24" style="26" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="26"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="30" t="s">
+        <v>298</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>297</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>295</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>296</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>328</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="31" t="s">
+        <v>300</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>234</v>
+      </c>
+      <c r="C2" s="53" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="53" t="s">
+        <v>124</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="31" t="s">
+        <v>299</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>235</v>
+      </c>
+      <c r="C3" s="53" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="53" t="s">
+        <v>125</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="31" t="s">
+        <v>301</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>236</v>
+      </c>
+      <c r="C4" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="53" t="s">
+        <v>127</v>
+      </c>
+      <c r="F4" s="32" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="32" t="s">
+        <v>292</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>237</v>
+      </c>
+      <c r="C5" s="53" t="s">
+        <v>218</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="53" t="s">
+        <v>129</v>
+      </c>
+      <c r="F5" s="32" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="31" t="s">
+        <v>319</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>238</v>
+      </c>
+      <c r="C6" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="53" t="s">
+        <v>131</v>
+      </c>
+      <c r="F6" s="32" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="31" t="s">
+        <v>315</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>239</v>
+      </c>
+      <c r="C7" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="53" t="s">
+        <v>232</v>
+      </c>
+      <c r="F7" s="32" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="31" t="s">
+        <v>306</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>240</v>
+      </c>
+      <c r="C8" s="53" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="53" t="s">
+        <v>133</v>
+      </c>
+      <c r="F8" s="32" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="31" t="s">
+        <v>302</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>241</v>
+      </c>
+      <c r="C9" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="53" t="s">
+        <v>135</v>
+      </c>
+      <c r="F9" s="32" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="31" t="s">
+        <v>304</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>242</v>
+      </c>
+      <c r="C10" s="53" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="53" t="s">
+        <v>136</v>
+      </c>
+      <c r="F10" s="32" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="33" t="s">
+        <v>327</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>243</v>
+      </c>
+      <c r="C11" s="53" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="53" t="s">
+        <v>140</v>
+      </c>
+      <c r="F11" s="32" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="31" t="s">
+        <v>311</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>244</v>
+      </c>
+      <c r="C12" s="53" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="53" t="s">
+        <v>138</v>
+      </c>
+      <c r="F12" s="32" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="33" t="s">
+        <v>308</v>
+      </c>
+      <c r="B13" s="32" t="s">
+        <v>245</v>
+      </c>
+      <c r="C13" s="53" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="53" t="s">
+        <v>226</v>
+      </c>
+      <c r="F13" s="32" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="31" t="s">
+        <v>303</v>
+      </c>
+      <c r="B14" s="32" t="s">
+        <v>246</v>
+      </c>
+      <c r="C14" s="53" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="53" t="s">
+        <v>141</v>
+      </c>
+      <c r="F14" s="32" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="32" t="s">
+        <v>293</v>
+      </c>
+      <c r="B15" s="32" t="s">
+        <v>247</v>
+      </c>
+      <c r="C15" s="53" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="53" t="s">
+        <v>143</v>
+      </c>
+      <c r="F15" s="32" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="31" t="s">
+        <v>307</v>
+      </c>
+      <c r="B16" s="32" t="s">
+        <v>248</v>
+      </c>
+      <c r="C16" s="53" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" s="53" t="s">
+        <v>145</v>
+      </c>
+      <c r="F16" s="32" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="31" t="s">
+        <v>312</v>
+      </c>
+      <c r="B17" s="32" t="s">
+        <v>249</v>
+      </c>
+      <c r="C17" s="53" t="s">
+        <v>231</v>
+      </c>
+      <c r="D17" s="32" t="s">
+        <v>230</v>
+      </c>
+      <c r="E17" s="53" t="s">
+        <v>147</v>
+      </c>
+      <c r="F17" s="32" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="31" t="s">
+        <v>320</v>
+      </c>
+      <c r="B18" s="32" t="s">
+        <v>250</v>
+      </c>
+      <c r="C18" s="53" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" s="53" t="s">
+        <v>150</v>
+      </c>
+      <c r="F18" s="32" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="33" t="s">
+        <v>322</v>
+      </c>
+      <c r="B19" s="32" t="s">
+        <v>251</v>
+      </c>
+      <c r="C19" s="53" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" s="53" t="s">
+        <v>151</v>
+      </c>
+      <c r="F19" s="32" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="31" t="s">
+        <v>305</v>
+      </c>
+      <c r="B20" s="32" t="s">
+        <v>252</v>
+      </c>
+      <c r="C20" s="53" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" s="53" t="s">
+        <v>153</v>
+      </c>
+      <c r="F20" s="32" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="31" t="s">
+        <v>321</v>
+      </c>
+      <c r="B21" s="32" t="s">
+        <v>253</v>
+      </c>
+      <c r="C21" s="53" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" s="53" t="s">
+        <v>224</v>
+      </c>
+      <c r="F21" s="32" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="32" t="s">
+        <v>294</v>
+      </c>
+      <c r="B22" s="32" t="s">
+        <v>254</v>
+      </c>
+      <c r="C22" s="53" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22" s="53" t="s">
+        <v>154</v>
+      </c>
+      <c r="F22" s="32" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="31" t="s">
+        <v>310</v>
+      </c>
+      <c r="B23" s="32" t="s">
+        <v>255</v>
+      </c>
+      <c r="C23" s="53" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="E23" s="53" t="s">
+        <v>156</v>
+      </c>
+      <c r="F23" s="32" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="34" t="s">
+        <v>309</v>
+      </c>
+      <c r="B24" s="32" t="s">
+        <v>256</v>
+      </c>
+      <c r="C24" s="53" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="E24" s="53" t="s">
+        <v>159</v>
+      </c>
+      <c r="F24" s="32" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="31" t="s">
+        <v>314</v>
+      </c>
+      <c r="B25" s="32" t="s">
+        <v>257</v>
+      </c>
+      <c r="C25" s="53" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" s="53" t="s">
+        <v>160</v>
+      </c>
+      <c r="F25" s="32" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="32" t="s">
+        <v>323</v>
+      </c>
+      <c r="B26" s="32" t="s">
+        <v>258</v>
+      </c>
+      <c r="C26" s="53" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" s="53" t="s">
+        <v>162</v>
+      </c>
+      <c r="F26" s="32" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="32" t="s">
+        <v>318</v>
+      </c>
+      <c r="B27" s="32" t="s">
+        <v>259</v>
+      </c>
+      <c r="C27" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="D27" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="53" t="s">
+        <v>164</v>
+      </c>
+      <c r="F27" s="32" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="32" t="s">
+        <v>317</v>
+      </c>
+      <c r="B28" s="32" t="s">
+        <v>260</v>
+      </c>
+      <c r="C28" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="E28" s="53" t="s">
+        <v>166</v>
+      </c>
+      <c r="F28" s="32" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="32" t="s">
+        <v>324</v>
+      </c>
+      <c r="B29" s="32" t="s">
+        <v>261</v>
+      </c>
+      <c r="C29" s="53" t="s">
+        <v>73</v>
+      </c>
+      <c r="D29" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="E29" s="53" t="s">
+        <v>168</v>
+      </c>
+      <c r="F29" s="32" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="31" t="s">
+        <v>313</v>
+      </c>
+      <c r="B30" s="32" t="s">
+        <v>262</v>
+      </c>
+      <c r="C30" s="53" t="s">
+        <v>75</v>
+      </c>
+      <c r="D30" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="E30" s="53" t="s">
+        <v>170</v>
+      </c>
+      <c r="F30" s="32" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="31" t="s">
+        <v>325</v>
+      </c>
+      <c r="B31" s="32" t="s">
+        <v>263</v>
+      </c>
+      <c r="C31" s="53" t="s">
+        <v>77</v>
+      </c>
+      <c r="D31" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="53" t="s">
+        <v>179</v>
+      </c>
+      <c r="F31" s="32" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="33" t="s">
+        <v>316</v>
+      </c>
+      <c r="B32" s="32" t="s">
+        <v>264</v>
+      </c>
+      <c r="C32" s="53" t="s">
+        <v>80</v>
+      </c>
+      <c r="D32" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" s="53" t="s">
+        <v>175</v>
+      </c>
+      <c r="F32" s="32" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="31" t="s">
+        <v>326</v>
+      </c>
+      <c r="B33" s="32" t="s">
+        <v>265</v>
+      </c>
+      <c r="C33" s="53" t="s">
+        <v>78</v>
+      </c>
+      <c r="D33" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" s="53" t="s">
+        <v>176</v>
+      </c>
+      <c r="F33" s="32" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="35"/>
+      <c r="B34" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="C34" s="53" t="s">
+        <v>79</v>
+      </c>
+      <c r="D34" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="53" t="s">
+        <v>182</v>
+      </c>
+      <c r="F34" s="32" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="32"/>
+      <c r="B35" s="32" t="s">
+        <v>267</v>
+      </c>
+      <c r="C35" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="D35" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="E35" s="53" t="s">
+        <v>172</v>
+      </c>
+      <c r="F35" s="32" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A36" s="32"/>
+      <c r="B36" s="32" t="s">
+        <v>268</v>
+      </c>
+      <c r="C36" s="53" t="s">
+        <v>85</v>
+      </c>
+      <c r="D36" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="E36" s="53" t="s">
+        <v>177</v>
+      </c>
+      <c r="F36" s="32" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="32"/>
+      <c r="B37" s="32" t="s">
+        <v>269</v>
+      </c>
+      <c r="C37" s="53" t="s">
+        <v>83</v>
+      </c>
+      <c r="D37" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" s="53" t="s">
+        <v>222</v>
+      </c>
+      <c r="F37" s="32" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="32"/>
+      <c r="B38" s="32" t="s">
+        <v>270</v>
+      </c>
+      <c r="C38" s="53" t="s">
+        <v>86</v>
+      </c>
+      <c r="D38" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="E38" s="53" t="s">
+        <v>183</v>
+      </c>
+      <c r="F38" s="32" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="32"/>
+      <c r="B39" s="32" t="s">
+        <v>271</v>
+      </c>
+      <c r="C39" s="53" t="s">
+        <v>88</v>
+      </c>
+      <c r="D39" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="E39" s="53" t="s">
+        <v>39</v>
+      </c>
+      <c r="F39" s="32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A40" s="32"/>
+      <c r="B40" s="32" t="s">
+        <v>272</v>
+      </c>
+      <c r="C40" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="D40" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="E40" s="53" t="s">
+        <v>185</v>
+      </c>
+      <c r="F40" s="32" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A41" s="32"/>
+      <c r="B41" s="32" t="s">
+        <v>273</v>
+      </c>
+      <c r="C41" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="D41" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="E41" s="53" t="s">
+        <v>219</v>
+      </c>
+      <c r="F41" s="32" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A42" s="32"/>
+      <c r="B42" s="32" t="s">
+        <v>274</v>
+      </c>
+      <c r="C42" s="53" t="s">
+        <v>94</v>
+      </c>
+      <c r="D42" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="E42" s="53" t="s">
+        <v>187</v>
+      </c>
+      <c r="F42" s="32" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A43" s="32"/>
+      <c r="B43" s="32" t="s">
+        <v>275</v>
+      </c>
+      <c r="C43" s="53" t="s">
+        <v>96</v>
+      </c>
+      <c r="D43" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="E43" s="53" t="s">
+        <v>189</v>
+      </c>
+      <c r="F43" s="32" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A44" s="32"/>
+      <c r="B44" s="32" t="s">
+        <v>276</v>
+      </c>
+      <c r="C44" s="53" t="s">
+        <v>99</v>
+      </c>
+      <c r="D44" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="E44" s="53" t="s">
+        <v>191</v>
+      </c>
+      <c r="F44" s="32" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A45" s="32"/>
+      <c r="B45" s="32" t="s">
+        <v>277</v>
+      </c>
+      <c r="C45" s="53" t="s">
+        <v>228</v>
+      </c>
+      <c r="D45" s="32" t="s">
+        <v>229</v>
+      </c>
+      <c r="E45" s="53" t="s">
+        <v>193</v>
+      </c>
+      <c r="F45" s="32" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A46" s="32"/>
+      <c r="B46" s="32" t="s">
+        <v>278</v>
+      </c>
+      <c r="C46" s="53" t="s">
+        <v>105</v>
+      </c>
+      <c r="D46" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="E46" s="53" t="s">
+        <v>194</v>
+      </c>
+      <c r="F46" s="32" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A47" s="32"/>
+      <c r="B47" s="32" t="s">
+        <v>279</v>
+      </c>
+      <c r="C47" s="53" t="s">
+        <v>109</v>
+      </c>
+      <c r="D47" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="E47" s="53" t="s">
+        <v>196</v>
+      </c>
+      <c r="F47" s="32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A48" s="32"/>
+      <c r="B48" s="32" t="s">
+        <v>280</v>
+      </c>
+      <c r="C48" s="53" t="s">
+        <v>115</v>
+      </c>
+      <c r="D48" s="32" t="s">
+        <v>114</v>
+      </c>
+      <c r="E48" s="53" t="s">
+        <v>197</v>
+      </c>
+      <c r="F48" s="32" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A49" s="32"/>
+      <c r="B49" s="32" t="s">
+        <v>281</v>
+      </c>
+      <c r="C49" s="53" t="s">
+        <v>118</v>
+      </c>
+      <c r="D49" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="E49" s="53" t="s">
+        <v>198</v>
+      </c>
+      <c r="F49" s="32" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A50" s="32"/>
+      <c r="B50" s="32" t="s">
+        <v>282</v>
+      </c>
+      <c r="C50" s="53" t="s">
+        <v>116</v>
+      </c>
+      <c r="D50" s="32" t="s">
+        <v>117</v>
+      </c>
+      <c r="E50" s="53" t="s">
+        <v>200</v>
+      </c>
+      <c r="F50" s="32" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A51" s="32"/>
+      <c r="B51" s="32" t="s">
+        <v>283</v>
+      </c>
+      <c r="C51" s="53" t="s">
+        <v>93</v>
+      </c>
+      <c r="D51" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="E51" s="53" t="s">
+        <v>202</v>
+      </c>
+      <c r="F51" s="32" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A52" s="32"/>
+      <c r="B52" s="32" t="s">
+        <v>284</v>
+      </c>
+      <c r="C52" s="53" t="s">
+        <v>97</v>
+      </c>
+      <c r="D52" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="E52" s="53" t="s">
+        <v>204</v>
+      </c>
+      <c r="F52" s="32" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A53" s="32"/>
+      <c r="B53" s="32" t="s">
+        <v>285</v>
+      </c>
+      <c r="C53" s="53" t="s">
+        <v>101</v>
+      </c>
+      <c r="D53" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="E53" s="53" t="s">
+        <v>207</v>
+      </c>
+      <c r="F53" s="32" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A54" s="32"/>
+      <c r="B54" s="32" t="s">
+        <v>286</v>
+      </c>
+      <c r="C54" s="53" t="s">
+        <v>103</v>
+      </c>
+      <c r="D54" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="E54" s="53" t="s">
+        <v>206</v>
+      </c>
+      <c r="F54" s="32" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A55" s="32"/>
+      <c r="B55" s="32" t="s">
+        <v>287</v>
+      </c>
+      <c r="C55" s="53" t="s">
+        <v>107</v>
+      </c>
+      <c r="D55" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="E55" s="53" t="s">
+        <v>212</v>
+      </c>
+      <c r="F55" s="32" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A56" s="32"/>
+      <c r="B56" s="32" t="s">
+        <v>288</v>
+      </c>
+      <c r="C56" s="53" t="s">
+        <v>111</v>
+      </c>
+      <c r="D56" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="E56" s="53" t="s">
+        <v>209</v>
+      </c>
+      <c r="F56" s="32" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A57" s="32"/>
+      <c r="B57" s="32" t="s">
+        <v>289</v>
+      </c>
+      <c r="C57" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="D57" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="E57" s="53" t="s">
+        <v>214</v>
+      </c>
+      <c r="F57" s="32" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A58" s="32"/>
+      <c r="B58" s="32" t="s">
+        <v>290</v>
+      </c>
+      <c r="C58" s="53" t="s">
+        <v>120</v>
+      </c>
+      <c r="D58" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="E58" s="53" t="s">
+        <v>215</v>
+      </c>
+      <c r="F58" s="32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A59" s="32"/>
+      <c r="B59" s="32" t="s">
+        <v>291</v>
+      </c>
+      <c r="C59" s="53" t="s">
+        <v>122</v>
+      </c>
+      <c r="D59" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="E59" s="53" t="s">
+        <v>221</v>
+      </c>
+      <c r="F59" s="32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A60" s="36"/>
+      <c r="B60" s="36"/>
+      <c r="C60" s="47"/>
+      <c r="D60" s="47"/>
+      <c r="E60" s="54" t="s">
+        <v>216</v>
+      </c>
+      <c r="F60" s="36" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A61" s="32"/>
+      <c r="B61" s="37"/>
+      <c r="C61" s="38"/>
+      <c r="D61" s="38"/>
+      <c r="E61" s="38"/>
+      <c r="F61" s="38"/>
+    </row>
+    <row r="62" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A62" s="29"/>
+      <c r="B62" s="27"/>
+    </row>
+    <row r="63" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A63" s="28"/>
+      <c r="B63" s="27"/>
+    </row>
+    <row r="64" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A64" s="28"/>
+      <c r="B64" s="27"/>
+    </row>
+    <row r="65" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A65" s="29"/>
+      <c r="B65" s="27"/>
+    </row>
+    <row r="66" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A66" s="28"/>
+      <c r="B66" s="27"/>
+    </row>
+    <row r="67" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A67" s="28"/>
+      <c r="B67" s="27"/>
+    </row>
+    <row r="68" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A68" s="28"/>
+      <c r="B68" s="27"/>
+    </row>
+    <row r="69" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A69" s="28"/>
+      <c r="B69" s="27"/>
+    </row>
+    <row r="70" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A70" s="28"/>
+      <c r="B70" s="27"/>
+    </row>
+    <row r="71" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A71" s="28"/>
+      <c r="B71" s="27"/>
+    </row>
+    <row r="72" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A72" s="28"/>
+      <c r="B72" s="27"/>
+    </row>
+    <row r="73" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A73" s="28"/>
+      <c r="B73" s="27"/>
+    </row>
+    <row r="74" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A74" s="28"/>
+      <c r="B74" s="27"/>
+    </row>
+    <row r="75" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A75" s="29"/>
+      <c r="B75" s="27"/>
+    </row>
+    <row r="76" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A76" s="28"/>
+      <c r="B76" s="27"/>
+    </row>
+    <row r="77" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A77" s="28"/>
+      <c r="B77" s="27"/>
+    </row>
+    <row r="78" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A78" s="28"/>
+      <c r="B78" s="27"/>
+    </row>
+    <row r="79" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A79" s="28"/>
+      <c r="B79" s="27"/>
+    </row>
+    <row r="80" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A80" s="28"/>
+      <c r="B80" s="27"/>
+    </row>
+    <row r="81" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A81" s="28"/>
+      <c r="B81" s="27"/>
+    </row>
+    <row r="82" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A82" s="28"/>
+      <c r="B82" s="27"/>
+    </row>
+    <row r="83" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A83" s="28"/>
+      <c r="B83" s="27"/>
+    </row>
+    <row r="84" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A84" s="28"/>
+      <c r="B84" s="27"/>
+    </row>
+    <row r="85" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A85" s="28"/>
+      <c r="B85" s="27"/>
+    </row>
+    <row r="86" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A86" s="28"/>
+      <c r="B86" s="27"/>
+    </row>
+    <row r="87" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A87" s="28"/>
+      <c r="B87" s="27"/>
+    </row>
+    <row r="88" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A88" s="28"/>
+      <c r="B88" s="27"/>
+    </row>
+    <row r="89" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A89" s="28"/>
+      <c r="B89" s="27"/>
+    </row>
+    <row r="90" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A90" s="28"/>
+      <c r="B90" s="27"/>
+    </row>
+    <row r="91" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A91" s="28"/>
+      <c r="B91" s="27"/>
+    </row>
+    <row r="92" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A92" s="28"/>
+      <c r="B92" s="27"/>
+    </row>
+    <row r="93" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A93" s="27"/>
+      <c r="B93" s="27"/>
+    </row>
+    <row r="94" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A94" s="27"/>
+      <c r="B94" s="27"/>
+    </row>
+    <row r="95" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A95" s="27"/>
+      <c r="B95" s="27"/>
+    </row>
+    <row r="96" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A96" s="27"/>
+      <c r="B96" s="27"/>
+    </row>
+    <row r="97" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A97" s="27"/>
+      <c r="B97" s="27"/>
+    </row>
+    <row r="98" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A98" s="27"/>
+      <c r="B98" s="27"/>
+    </row>
+    <row r="99" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A99" s="27"/>
+      <c r="B99" s="27"/>
+    </row>
+    <row r="100" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A100" s="27"/>
+      <c r="B100" s="27"/>
+    </row>
+    <row r="101" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A101" s="27"/>
+      <c r="B101" s="27"/>
+    </row>
+    <row r="102" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A102" s="27"/>
+      <c r="B102" s="27"/>
+    </row>
+    <row r="103" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A103" s="27"/>
+      <c r="B103" s="27"/>
+    </row>
+    <row r="104" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A104" s="27"/>
+      <c r="B104" s="27"/>
+    </row>
+    <row r="105" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A105" s="27"/>
+      <c r="B105" s="27"/>
+    </row>
+    <row r="106" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A106" s="27"/>
+      <c r="B106" s="27"/>
+    </row>
+    <row r="107" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A107" s="27"/>
+      <c r="B107" s="27"/>
+    </row>
+    <row r="108" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A108" s="27"/>
+      <c r="B108" s="27"/>
+    </row>
+    <row r="109" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A109" s="27"/>
+      <c r="B109" s="27"/>
+    </row>
+    <row r="110" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A110" s="27"/>
+      <c r="B110" s="27"/>
+    </row>
+    <row r="111" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A111" s="27"/>
+      <c r="B111" s="27"/>
+    </row>
+    <row r="112" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A112" s="27"/>
+      <c r="B112" s="27"/>
+    </row>
+    <row r="113" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A113" s="27"/>
+      <c r="B113" s="27"/>
+    </row>
+    <row r="114" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A114" s="27"/>
+      <c r="B114" s="27"/>
+    </row>
+    <row r="115" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A115" s="27"/>
+      <c r="B115" s="27"/>
+    </row>
+    <row r="116" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A116" s="27"/>
+      <c r="B116" s="27"/>
+    </row>
+    <row r="117" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A117" s="27"/>
+      <c r="B117" s="27"/>
+    </row>
+    <row r="118" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A118" s="27"/>
+      <c r="B118" s="27"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="40" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B68"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="42.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="39.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="30" t="s">
+        <v>298</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="55" t="s">
+        <v>300</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="55" t="s">
+        <v>299</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="55" t="s">
+        <v>301</v>
+      </c>
+      <c r="B4" s="53" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="31" t="s">
+        <v>385</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="31" t="s">
+        <v>386</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="55" t="s">
+        <v>315</v>
+      </c>
+      <c r="B7" s="53" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="55" t="s">
+        <v>306</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="55" t="s">
+        <v>302</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="55" t="s">
+        <v>304</v>
+      </c>
+      <c r="B10" s="53" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="33" t="s">
+        <v>387</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="55" t="s">
+        <v>311</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="56" t="s">
+        <v>308</v>
+      </c>
+      <c r="B13" s="53" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="55" t="s">
+        <v>303</v>
+      </c>
+      <c r="B14" s="32" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="53" t="s">
+        <v>330</v>
+      </c>
+      <c r="B15" s="32" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="55" t="s">
+        <v>307</v>
+      </c>
+      <c r="B16" s="32" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="55" t="s">
+        <v>312</v>
+      </c>
+      <c r="B17" s="32" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="55" t="s">
+        <v>320</v>
+      </c>
+      <c r="B18" s="32" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="33" t="s">
+        <v>388</v>
+      </c>
+      <c r="B19" s="32" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="55" t="s">
+        <v>305</v>
+      </c>
+      <c r="B20" s="53" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="31" t="s">
+        <v>389</v>
+      </c>
+      <c r="B21" s="32" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="31" t="s">
+        <v>355</v>
+      </c>
+      <c r="B22" s="32" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="55" t="s">
+        <v>310</v>
+      </c>
+      <c r="B23" s="53" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="34" t="s">
+        <v>390</v>
+      </c>
+      <c r="B24" s="53" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="31" t="s">
+        <v>314</v>
+      </c>
+      <c r="B25" s="53" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="53" t="s">
+        <v>323</v>
+      </c>
+      <c r="B26" s="53" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="53" t="s">
+        <v>318</v>
+      </c>
+      <c r="B27" s="53" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="53" t="s">
+        <v>317</v>
+      </c>
+      <c r="B28" s="53" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="53" t="s">
+        <v>324</v>
+      </c>
+      <c r="B29" s="53" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="31" t="s">
+        <v>313</v>
+      </c>
+      <c r="B30" s="53" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="31" t="s">
+        <v>391</v>
+      </c>
+      <c r="B31" s="53" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="56" t="s">
+        <v>316</v>
+      </c>
+      <c r="B32" s="53" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="55" t="s">
+        <v>326</v>
+      </c>
+      <c r="B33" s="32" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="32"/>
+      <c r="B34" s="53" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="32"/>
+      <c r="B35" s="53" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A36" s="32"/>
+      <c r="B36" s="53" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="32"/>
+      <c r="B37" s="53" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="32"/>
+      <c r="B38" s="32" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="32"/>
+      <c r="B39" s="53" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A40" s="32"/>
+      <c r="B40" s="53" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A41" s="32"/>
+      <c r="B41" s="32" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A42" s="32"/>
+      <c r="B42" s="32" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A43" s="32"/>
+      <c r="B43" s="32" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A44" s="32"/>
+      <c r="B44" s="53" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A45" s="32"/>
+      <c r="B45" s="32" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A46" s="32"/>
+      <c r="B46" s="53" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A47" s="32"/>
+      <c r="B47" s="53" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A48" s="32"/>
+      <c r="B48" s="53" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A49" s="32"/>
+      <c r="B49" s="32" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A50" s="32"/>
+      <c r="B50" s="53" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A51" s="32"/>
+      <c r="B51" s="53" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A52" s="32"/>
+      <c r="B52" s="53" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A53" s="32"/>
+      <c r="B53" s="53" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A54" s="32"/>
+      <c r="B54" s="32" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A55" s="32"/>
+      <c r="B55" s="32" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A56" s="32"/>
+      <c r="B56" s="32" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A57" s="32"/>
+      <c r="B57" s="37" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A58" s="32"/>
+      <c r="B58" s="32" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A59" s="32"/>
+      <c r="B59" s="32" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A60" s="32"/>
+      <c r="B60" s="53" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A61" s="32"/>
+      <c r="B61" s="32" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A62" s="32"/>
+      <c r="B62" s="32" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A63" s="32"/>
+      <c r="B63" s="53" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A64" s="32"/>
+      <c r="B64" s="32" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A65" s="32"/>
+      <c r="B65" s="53" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A66" s="32"/>
+      <c r="B66" s="53" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A67" s="32"/>
+      <c r="B67" s="32" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A68" s="36"/>
+      <c r="B68" s="54" t="s">
+        <v>291</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>